<commit_message>
added to rmarkdown code, changed the surv variable so it wasn't duplicated. added figures and text to conditioning period. ran the 'match' version with apportionments 1:9 and 11.
</commit_message>
<xml_diff>
--- a/data/Sablefish_Input_matchMGMTqselex.xlsx
+++ b/data/Sablefish_Input_matchMGMTqselex.xlsx
@@ -27416,7 +27416,7 @@
         <v>66</v>
       </c>
       <c r="B2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -27449,7 +27449,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -27460,7 +27460,7 @@
         <v>128</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>129</v>

</xml_diff>